<commit_message>
Fix: last packer plan + add skus
</commit_message>
<xml_diff>
--- a/app/data/static/params/brynza.xlsx
+++ b/app/data/static/params/brynza.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
   <si>
     <t xml:space="preserve">Название SKU</t>
   </si>
@@ -98,6 +98,15 @@
   </si>
   <si>
     <t xml:space="preserve">00-00010095</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Брынза классическая "Из Лавки", 45%, 0,2 кг, т/ф</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Из Лавки</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00-00012173</t>
   </si>
 </sst>
 </file>
@@ -107,7 +116,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -143,6 +152,12 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -194,7 +209,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -208,6 +223,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -228,10 +251,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K7" activeCellId="0" sqref="K7"/>
+      <selection pane="topLeft" activeCell="K21" activeCellId="0" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -482,6 +505,41 @@
         <v>25</v>
       </c>
     </row>
+    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>350</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>